<commit_message>
created a UK on reg_id field and updated the DD for reg client DB
</commit_message>
<xml_diff>
--- a/scripts/database/data_model/mosip_reg_dd.xlsx
+++ b/scripts/database/data_model/mosip_reg_dd.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Backup\NasirKhan\MindTree\Digital\Projects\MOSIP\Data Model\DataDictionary\Latest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\mosip\scripts\database\data_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FAE4CAE-EE0F-4B20-B501-2CD052665026}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DF9DD0D2-4640-453F-83DD-B6A02CA790D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9314" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9314" uniqueCount="683">
   <si>
     <t>app_id</t>
   </si>
@@ -2004,6 +2004,78 @@
   </si>
   <si>
     <t>Key Index: Fingerprint[Unique Hash ]  for the TPM public key</t>
+  </si>
+  <si>
+    <t>Audit Log Control : Control table to manage audit log sync from registration client to audit server. The sync process takes place as part of registration packet upload process.</t>
+  </si>
+  <si>
+    <t>Individual Type: Master list of individual type who are allowed for registration to get UIN.Eg. Foreigner, Non-Foreigner..etc</t>
+  </si>
+  <si>
+    <t>Pre Registration List : List of pre registration data that are download at registration client application for processing.</t>
+  </si>
+  <si>
+    <t>Pre registration ID: ID whicg is dowloaded from pre-registration apllication for processing</t>
+  </si>
+  <si>
+    <t>Packet Symmetric Key : Symmetric used to encrypt the data while receiving the packets from pre registration application.</t>
+  </si>
+  <si>
+    <t>Registration: Stores all the registration request of an individual along with other details that are needed to process the registration request. This also keeps track of registration process status of an individual.</t>
+  </si>
+  <si>
+    <t>ID: Registration ID of an individual request to proccess for a UIN or to update details of UIN</t>
+  </si>
+  <si>
+    <t>Registration Type: Type of an registration eg. New, Update or Correction</t>
+  </si>
+  <si>
+    <t>Reference Registration ID: Previous registration ID using which UIN was generated, Which will be used as refrence for any update or correction request.</t>
+  </si>
+  <si>
+    <t>Pre registration ID: ID of the pre registation application that was used to create this registration request.</t>
+  </si>
+  <si>
+    <t>Status Code: Status of the registration process, This will be the over all status of the registration</t>
+  </si>
+  <si>
+    <t>Client Status Code : Status which is tracked within client application of a registration process..eg.end of the day approval by supervisor…etc</t>
+  </si>
+  <si>
+    <t>Server Status Code : Status code as received from the registration processor for the registration request..eg.packet approved, packet resend…etc</t>
+  </si>
+  <si>
+    <t>Registration User ID : User ID of the registration officer who created the registration request</t>
+  </si>
+  <si>
+    <t>Registration Center ID : ID of the registration center where the registration request is created</t>
+  </si>
+  <si>
+    <t>Approver User ID : User ID of the registration officer/supervisor who approved the registration/packets.</t>
+  </si>
+  <si>
+    <t>Approver Role Code : Role of the user who approved registration/packets….eg. registation officer, supervisor…etc.</t>
+  </si>
+  <si>
+    <t>Latest Registration Transaction ID : Transaction ID of the last client side transaction that was executed for this registration request. This can be used to handle/track transactions of an registration request.</t>
+  </si>
+  <si>
+    <t>Latest Transaction Type Code : Transaction Type code of the last client side transaction that was executed for this registration request</t>
+  </si>
+  <si>
+    <t>Latest Transaction Status Code: Transaction status code of the last client side transaction that was executed for this registration request</t>
+  </si>
+  <si>
+    <t>Latest Transaction Language Code : Transaction language code of the last client side transaction that was executed for this registration request</t>
+  </si>
+  <si>
+    <t>Latest Registration Transaction date and time : Date and time of last Transaction of the last client side transaction that was executed for this registration request</t>
+  </si>
+  <si>
+    <t>Registration Sequence ID: Maintains latest sequence number available to generate registration id in every client machine.</t>
+  </si>
+  <si>
+    <t>User Biometric : Stores all user biomentric specific information in machine at registration center to authenticate users.</t>
   </si>
 </sst>
 </file>
@@ -2412,9 +2484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB01DA9-233F-41B5-BD9F-67EB46FB1578}">
   <dimension ref="B1:J761"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4184,7 +4254,7 @@
         <v>88</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>582</v>
+        <v>659</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5">
@@ -8077,7 +8147,7 @@
         <v>188</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>595</v>
+        <v>660</v>
       </c>
       <c r="D234" s="5"/>
       <c r="E234" s="5">
@@ -10422,7 +10492,7 @@
         <v>252</v>
       </c>
       <c r="C331" s="5" t="s">
-        <v>602</v>
+        <v>661</v>
       </c>
       <c r="D331" s="5"/>
       <c r="E331" s="5">
@@ -10471,7 +10541,7 @@
         <v>255</v>
       </c>
       <c r="D333" s="7" t="s">
-        <v>256</v>
+        <v>662</v>
       </c>
       <c r="E333" s="7">
         <v>2</v>
@@ -10569,7 +10639,7 @@
         <v>264</v>
       </c>
       <c r="D337" s="7" t="s">
-        <v>265</v>
+        <v>663</v>
       </c>
       <c r="E337" s="7">
         <v>6</v>
@@ -13521,7 +13591,7 @@
         <v>331</v>
       </c>
       <c r="C458" s="5" t="s">
-        <v>612</v>
+        <v>664</v>
       </c>
       <c r="D458" s="5"/>
       <c r="E458" s="5">
@@ -13541,7 +13611,7 @@
         <v>69</v>
       </c>
       <c r="D459" s="7" t="s">
-        <v>333</v>
+        <v>665</v>
       </c>
       <c r="E459" s="7">
         <v>1</v>
@@ -13570,7 +13640,7 @@
         <v>334</v>
       </c>
       <c r="D460" s="7" t="s">
-        <v>335</v>
+        <v>666</v>
       </c>
       <c r="E460" s="7">
         <v>2</v>
@@ -13595,7 +13665,7 @@
         <v>336</v>
       </c>
       <c r="D461" s="7" t="s">
-        <v>337</v>
+        <v>667</v>
       </c>
       <c r="E461" s="7">
         <v>3</v>
@@ -13620,7 +13690,7 @@
         <v>255</v>
       </c>
       <c r="D462" s="7" t="s">
-        <v>338</v>
+        <v>668</v>
       </c>
       <c r="E462" s="7">
         <v>4</v>
@@ -13645,7 +13715,7 @@
         <v>203</v>
       </c>
       <c r="D463" s="7" t="s">
-        <v>339</v>
+        <v>669</v>
       </c>
       <c r="E463" s="7">
         <v>5</v>
@@ -13772,7 +13842,7 @@
         <v>346</v>
       </c>
       <c r="D468" s="7" t="s">
-        <v>347</v>
+        <v>670</v>
       </c>
       <c r="E468" s="7">
         <v>10</v>
@@ -13797,7 +13867,7 @@
         <v>348</v>
       </c>
       <c r="D469" s="7" t="s">
-        <v>349</v>
+        <v>671</v>
       </c>
       <c r="E469" s="7">
         <v>11</v>
@@ -13918,7 +13988,7 @@
         <v>358</v>
       </c>
       <c r="D474" s="7" t="s">
-        <v>360</v>
+        <v>672</v>
       </c>
       <c r="E474" s="7">
         <v>16</v>
@@ -13947,7 +14017,7 @@
         <v>295</v>
       </c>
       <c r="D475" s="7" t="s">
-        <v>361</v>
+        <v>673</v>
       </c>
       <c r="E475" s="7">
         <v>17</v>
@@ -13976,7 +14046,7 @@
         <v>362</v>
       </c>
       <c r="D476" s="7" t="s">
-        <v>364</v>
+        <v>674</v>
       </c>
       <c r="E476" s="7">
         <v>18</v>
@@ -14005,7 +14075,7 @@
         <v>365</v>
       </c>
       <c r="D477" s="7" t="s">
-        <v>366</v>
+        <v>675</v>
       </c>
       <c r="E477" s="7">
         <v>19</v>
@@ -14101,7 +14171,7 @@
         <v>371</v>
       </c>
       <c r="D481" s="7" t="s">
-        <v>372</v>
+        <v>676</v>
       </c>
       <c r="E481" s="7">
         <v>23</v>
@@ -14126,7 +14196,7 @@
         <v>373</v>
       </c>
       <c r="D482" s="7" t="s">
-        <v>374</v>
+        <v>677</v>
       </c>
       <c r="E482" s="7">
         <v>24</v>
@@ -14151,7 +14221,7 @@
         <v>375</v>
       </c>
       <c r="D483" s="7" t="s">
-        <v>376</v>
+        <v>678</v>
       </c>
       <c r="E483" s="7">
         <v>25</v>
@@ -14176,7 +14246,7 @@
         <v>377</v>
       </c>
       <c r="D484" s="7" t="s">
-        <v>378</v>
+        <v>679</v>
       </c>
       <c r="E484" s="7">
         <v>26</v>
@@ -14201,7 +14271,7 @@
         <v>379</v>
       </c>
       <c r="D485" s="7" t="s">
-        <v>380</v>
+        <v>680</v>
       </c>
       <c r="E485" s="7">
         <v>27</v>
@@ -15418,7 +15488,7 @@
         <v>434</v>
       </c>
       <c r="C535" s="5" t="s">
-        <v>615</v>
+        <v>681</v>
       </c>
       <c r="D535" s="5"/>
       <c r="E535" s="5">
@@ -19210,7 +19280,7 @@
         <v>527</v>
       </c>
       <c r="C691" s="5" t="s">
-        <v>625</v>
+        <v>682</v>
       </c>
       <c r="D691" s="5"/>
       <c r="E691" s="5">

</xml_diff>